<commit_message>
update landusebuff function; push to scripts
</commit_message>
<xml_diff>
--- a/PPA2/Input_Template/XLSX/PPA_Template_SGR_CS.xlsx
+++ b/PPA2/Input_Template/XLSX/PPA_Template_SGR_CS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\arcserver-svr\D\PPA_v2_SVR\PPA2\Input_Template\XLSX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\ProjectLevelPerformanceAssessment\PPAv2\PPA2_0_code\PPA2\Input_Template\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146F0653-3CB6-4614-80AA-191CB84A9747}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C71EDC9-306A-4A8F-8403-6FFB961EBA13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="495" windowWidth="22815" windowHeight="13080" tabRatio="781" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" tabRatio="781" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0ATitlePg" sheetId="4" r:id="rId1"/>
@@ -49,7 +49,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -3002,433 +3004,6 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Entry-Level Job Accessibility for EJ Populations </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Adjacent to Project</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>lookup_helper!$B$100:$B$103</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>30-min walk</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30-min biking</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30-min drive</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>45-min transit</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>lookup_helper!$D$100:$D$103</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>272.66024096385541</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>795.25333333333333</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12386.82514056225</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1514.9185542168671</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E5E3-46E9-A4BB-CF4983A9EDA5}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1587649183"/>
-        <c:axId val="1544029663"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1587649183"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-2160000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1544029663"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1544029663"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Destinations</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1587649183"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
               <a:t>Education</a:t>
             </a:r>
             <a:r>
@@ -3829,7 +3404,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4264,7 +3839,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -9887,46 +9462,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -12260,509 +11795,6 @@
 </file>
 
 <file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -17686,22 +16718,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>57151</xdr:colOff>
+      <xdr:colOff>57147</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>85726</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>47626</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>161926</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>685797</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{486BF543-A7FF-4787-BAD3-3676364CE88E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE6DEDB4-1421-452B-82AE-DFC951CAEAC0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17724,53 +16756,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>76201</xdr:colOff>
+      <xdr:colOff>61910</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>4764</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
+      <xdr:colOff>33335</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE6DEDB4-1421-452B-82AE-DFC951CAEAC0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>47626</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>90488</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17791,7 +16785,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -18143,9 +17137,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18408,9 +17400,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
+    <sheetView view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18532,23 +17522,25 @@
         <v>258</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="99" t="s">
+    <row r="72" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="99" t="s">
         <v>237</v>
       </c>
-      <c r="B86" s="99"/>
-      <c r="C86" s="99"/>
-      <c r="D86" s="99"/>
-      <c r="E86" s="99"/>
-      <c r="F86" s="99"/>
-      <c r="G86" s="99"/>
+      <c r="B72" s="99"/>
+      <c r="C72" s="99"/>
+      <c r="D72" s="99"/>
+      <c r="E72" s="99"/>
+      <c r="F72" s="99"/>
+      <c r="G72" s="99"/>
+    </row>
+    <row r="86" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H86" s="65"/>
       <c r="I86" s="65"/>
     </row>
-    <row r="90" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="8:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A86:G86"/>
+    <mergeCell ref="A72:G72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="96" orientation="portrait" r:id="rId1"/>
@@ -24541,7 +23533,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:H2"/>
     </sheetView>
   </sheetViews>
@@ -24766,8 +23758,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A31" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24776,8 +23768,9 @@
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="5" width="6.5703125" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix K-12 enrollment count error in CS spreadsheet
Was a hard-coded value when it should have been a lookup to the lookup_helper tab.
</commit_message>
<xml_diff>
--- a/PPA2/Input_Template/XLSX/PPA_Template_SGR_CS.xlsx
+++ b/PPA2/Input_Template/XLSX/PPA_Template_SGR_CS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\ProjectLevelPerformanceAssessment\PPAv2\PPA2_0_code\PPA2\Input_Template\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D854A00E-1578-4E5E-9507-EAD58C232238}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA17D199-0F72-417B-989F-2F9333F19C68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="781" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1888,7 +1888,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2008,6 +2007,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -17592,40 +17592,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="96" t="str">
+      <c r="A2" s="95" t="str">
         <f>"Project Performance Assessment Report: "&amp;import!$B$2</f>
         <v>Project Performance Assessment Report: test_project_YubaCity</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="96"/>
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
+      <c r="A3" s="95"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="96"/>
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
+      <c r="A4" s="95"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -17638,84 +17638,84 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="95" t="s">
+      <c r="A31" s="94" t="s">
         <v>129</v>
       </c>
-      <c r="B31" s="95"/>
-      <c r="C31" s="95"/>
-      <c r="D31" s="95"/>
+      <c r="B31" s="94"/>
+      <c r="C31" s="94"/>
+      <c r="D31" s="94"/>
       <c r="E31" s="31" t="str">
         <f>VLOOKUP(A31,lookup_helper!$B$112:$D$119,3,FALSE)</f>
         <v>test_project_YubaCity</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="69" t="s">
+      <c r="A32" s="68" t="s">
         <v>281</v>
       </c>
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69"/>
+      <c r="B32" s="68"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="68"/>
       <c r="E32" s="31" t="str">
         <f>VLOOKUP(A32,lookup_helper!$B$112:$D$119,3,FALSE)</f>
         <v>anyplace</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="95" t="s">
+      <c r="A33" s="94" t="s">
         <v>130</v>
       </c>
-      <c r="B33" s="95"/>
-      <c r="C33" s="95"/>
-      <c r="D33" s="95"/>
+      <c r="B33" s="94"/>
+      <c r="C33" s="94"/>
+      <c r="D33" s="94"/>
       <c r="E33" s="31" t="str">
         <f>VLOOKUP(A33,lookup_helper!$B$112:$D$119,3,FALSE)</f>
         <v>Freeway</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="95" t="s">
+      <c r="A34" s="94" t="s">
         <v>131</v>
       </c>
-      <c r="B34" s="95"/>
-      <c r="C34" s="95"/>
-      <c r="D34" s="95"/>
+      <c r="B34" s="94"/>
+      <c r="C34" s="94"/>
+      <c r="D34" s="94"/>
       <c r="E34" s="32">
         <f>VLOOKUP(A34,lookup_helper!$B$112:$D$119,3,FALSE)</f>
         <v>60000</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="95" t="s">
+      <c r="A35" s="94" t="s">
         <v>132</v>
       </c>
-      <c r="B35" s="95"/>
-      <c r="C35" s="95"/>
-      <c r="D35" s="95"/>
+      <c r="B35" s="94"/>
+      <c r="C35" s="94"/>
+      <c r="D35" s="94"/>
       <c r="E35" s="32">
         <f>VLOOKUP(A35,lookup_helper!$B$112:$D$119,3,FALSE)</f>
         <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="95" t="s">
+      <c r="A36" s="94" t="s">
         <v>133</v>
       </c>
-      <c r="B36" s="95"/>
-      <c r="C36" s="95"/>
-      <c r="D36" s="95"/>
+      <c r="B36" s="94"/>
+      <c r="C36" s="94"/>
+      <c r="D36" s="94"/>
       <c r="E36" s="32">
         <f>VLOOKUP(A36,lookup_helper!$B$112:$D$119,3,FALSE)</f>
         <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="95" t="s">
+      <c r="A37" s="94" t="s">
         <v>251</v>
       </c>
-      <c r="B37" s="95"/>
-      <c r="C37" s="95"/>
-      <c r="D37" s="95"/>
+      <c r="B37" s="94"/>
+      <c r="C37" s="94"/>
+      <c r="D37" s="94"/>
       <c r="E37" s="48">
         <f>VLOOKUP(A37,lookup_helper!$B$112:$D$119,3,FALSE)</f>
         <v>1.41</v>
@@ -17726,12 +17726,12 @@
       <c r="I37" s="30"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="95" t="s">
+      <c r="A38" s="94" t="s">
         <v>134</v>
       </c>
-      <c r="B38" s="95"/>
-      <c r="C38" s="95"/>
-      <c r="D38" s="95"/>
+      <c r="B38" s="94"/>
+      <c r="C38" s="94"/>
+      <c r="D38" s="94"/>
       <c r="E38" s="31" t="str">
         <f>VLOOKUP(A38,lookup_helper!$B$112:$D$119,3,FALSE)</f>
         <v>Small-Town Established Communities</v>
@@ -17786,7 +17786,7 @@
       <c r="I42" s="11"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="56" t="s">
+      <c r="A43" s="55" t="s">
         <v>303</v>
       </c>
       <c r="B43" s="11"/>
@@ -17799,7 +17799,7 @@
       <c r="I43" s="11"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="94"/>
+      <c r="A44" s="93"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
       <c r="D44" s="11"/>
@@ -17856,20 +17856,20 @@
     <col min="7" max="7" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H1" s="68" t="str">
+    <row r="1" spans="1:8" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="67" t="str">
         <f>"Project name: "&amp;VLOOKUP("Project name",lookup_helper!$B:$D,3,FALSE)</f>
         <v>Project name: test_project_YubaCity</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H2" s="68" t="str">
+    <row r="2" spans="1:8" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="67" t="str">
         <f>"Project community type: "&amp;VLOOKUP("Project Community Type",lookup_helper!$B:$D,3,FALSE)</f>
         <v>Project community type: Small-Town Established Communities</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
+      <c r="A3" s="58"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -17962,24 +17962,24 @@
       <c r="E21" s="51"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="67" t="s">
+      <c r="A34" s="66" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="99" t="s">
+      <c r="A72" s="98" t="s">
         <v>237</v>
       </c>
-      <c r="B72" s="99"/>
-      <c r="C72" s="99"/>
-      <c r="D72" s="99"/>
-      <c r="E72" s="99"/>
-      <c r="F72" s="99"/>
-      <c r="G72" s="99"/>
+      <c r="B72" s="98"/>
+      <c r="C72" s="98"/>
+      <c r="D72" s="98"/>
+      <c r="E72" s="98"/>
+      <c r="F72" s="98"/>
+      <c r="G72" s="98"/>
     </row>
     <row r="86" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H86" s="65"/>
-      <c r="I86" s="65"/>
+      <c r="H86" s="64"/>
+      <c r="I86" s="64"/>
     </row>
     <row r="90" spans="8:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -18001,9 +18001,9 @@
   <dimension ref="A1:G117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B110" sqref="B110"/>
-      <selection pane="bottomLeft" activeCell="B110" sqref="B110"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18702,7 +18702,7 @@
       <c r="A68" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B68" s="77">
+      <c r="B68" s="76">
         <v>1.3624389724527719</v>
       </c>
       <c r="D68" s="5">
@@ -18716,7 +18716,7 @@
       <c r="A69" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B69" s="77">
+      <c r="B69" s="76">
         <v>1.475654647382425</v>
       </c>
       <c r="D69" s="5">
@@ -19238,7 +19238,7 @@
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B110" sqref="B110"/>
-      <selection pane="bottomLeft" activeCell="B110" sqref="B110"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19958,14 +19958,14 @@
         <f>VLOOKUP($A18,import!$A:$G,MATCH(lookup_helper!I$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
-      <c r="P18" s="63" t="s">
+      <c r="P18" s="62" t="s">
         <v>274</v>
       </c>
-      <c r="Q18" s="61">
+      <c r="Q18" s="60">
         <f t="array" ref="Q18">MAX(IF(ISNUMBER(SEARCH("calc_len",import!$A:$A)),import!$B:$B))</f>
         <v>7460.2525126827086</v>
       </c>
-      <c r="R18" s="62"/>
+      <c r="R18" s="61"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -20004,10 +20004,10 @@
       <c r="J19" t="s">
         <v>170</v>
       </c>
-      <c r="P19" s="60" t="s">
+      <c r="P19" s="59" t="s">
         <v>273</v>
       </c>
-      <c r="Q19" s="64">
+      <c r="Q19" s="63">
         <f>(Q18/5280)/D118</f>
         <v>1.0020756115251865</v>
       </c>
@@ -21596,19 +21596,19 @@
       <c r="C63" t="s">
         <v>216</v>
       </c>
-      <c r="D63" s="91">
+      <c r="D63" s="90">
         <f>VLOOKUP($A63,import!$A:$G,MATCH(lookup_helper!D$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>13.047842643653521</v>
       </c>
-      <c r="E63" s="91">
+      <c r="E63" s="90">
         <f>VLOOKUP($A63,import!$A:$G,MATCH(lookup_helper!E$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>69.301955921047991</v>
       </c>
-      <c r="F63" s="91">
+      <c r="F63" s="90">
         <f>VLOOKUP($A63,import!$A:$G,MATCH(lookup_helper!F$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G63" s="91">
+      <c r="G63" s="90">
         <f>VLOOKUP($A63,import!$A:$G,MATCH(lookup_helper!G$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
@@ -21656,37 +21656,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" s="85" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="85" t="s">
+    <row r="65" spans="1:9" s="84" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="B65" s="84" t="s">
+      <c r="B65" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="C65" s="85" t="s">
+      <c r="C65" s="84" t="s">
         <v>208</v>
       </c>
-      <c r="D65" s="83">
+      <c r="D65" s="82">
         <f>VLOOKUP($A65,import!$A:$G,MATCH(lookup_helper!D$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>1175.845221386116</v>
       </c>
-      <c r="E65" s="83">
+      <c r="E65" s="82">
         <f>VLOOKUP($A65,import!$A:$G,MATCH(lookup_helper!E$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
-      <c r="F65" s="83">
+      <c r="F65" s="82">
         <f>VLOOKUP($A65,import!$A:$G,MATCH(lookup_helper!F$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G65" s="83">
+      <c r="G65" s="82">
         <f>VLOOKUP($A65,import!$A:$G,MATCH(lookup_helper!G$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
-      <c r="H65" s="85">
+      <c r="H65" s="84">
         <f>VLOOKUP($A65,import!$A:$G,MATCH(lookup_helper!H$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I65" s="85">
+      <c r="I65" s="84">
         <f>VLOOKUP($A65,import!$A:$G,MATCH(lookup_helper!I$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
@@ -22181,72 +22181,72 @@
         <v>0.93085349575304976</v>
       </c>
     </row>
-    <row r="80" spans="1:9" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="85" t="s">
+    <row r="80" spans="1:9" s="84" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="B80" s="84" t="s">
+      <c r="B80" s="83" t="s">
         <v>185</v>
       </c>
-      <c r="C80" s="85" t="s">
+      <c r="C80" s="84" t="s">
         <v>213</v>
       </c>
-      <c r="D80" s="83">
+      <c r="D80" s="82">
         <f>VLOOKUP($A80,import!$A:$G,MATCH(lookup_helper!D$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>1916</v>
       </c>
-      <c r="E80" s="83">
+      <c r="E80" s="82">
         <f>VLOOKUP($A80,import!$A:$G,MATCH(lookup_helper!E$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>2072.611115859987</v>
       </c>
-      <c r="F80" s="85">
+      <c r="F80" s="84">
         <f>VLOOKUP($A80,import!$A:$G,MATCH(lookup_helper!F$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G80" s="85">
+      <c r="G80" s="84">
         <f>VLOOKUP($A80,import!$A:$G,MATCH(lookup_helper!G$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
-      <c r="H80" s="85">
+      <c r="H80" s="84">
         <f>VLOOKUP($A80,import!$A:$G,MATCH(lookup_helper!H$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I80" s="85">
+      <c r="I80" s="84">
         <f>VLOOKUP($A80,import!$A:$G,MATCH(lookup_helper!I$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:16" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="85" t="s">
+    <row r="81" spans="1:16" s="84" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="84" t="s">
         <v>89</v>
       </c>
-      <c r="B81" s="84" t="s">
+      <c r="B81" s="83" t="s">
         <v>183</v>
       </c>
-      <c r="C81" s="85" t="s">
+      <c r="C81" s="84" t="s">
         <v>213</v>
       </c>
-      <c r="D81" s="83">
+      <c r="D81" s="82">
         <f>VLOOKUP($A81,import!$A:$G,MATCH(lookup_helper!D$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>1769</v>
       </c>
-      <c r="E81" s="83">
+      <c r="E81" s="82">
         <f>VLOOKUP($A81,import!$A:$G,MATCH(lookup_helper!E$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>2761.6599999999989</v>
       </c>
-      <c r="F81" s="85">
+      <c r="F81" s="84">
         <f>VLOOKUP($A81,import!$A:$G,MATCH(lookup_helper!F$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
-      <c r="G81" s="85">
+      <c r="G81" s="84">
         <f>VLOOKUP($A81,import!$A:$G,MATCH(lookup_helper!G$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
-      <c r="H81" s="85">
+      <c r="H81" s="84">
         <f>VLOOKUP($A81,import!$A:$G,MATCH(lookup_helper!H$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I81" s="85">
+      <c r="I81" s="84">
         <f>VLOOKUP($A81,import!$A:$G,MATCH(lookup_helper!I$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
@@ -22286,72 +22286,72 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:16" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="83" t="s">
+    <row r="83" spans="1:16" s="84" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="82" t="s">
         <v>65</v>
       </c>
-      <c r="B83" s="84" t="s">
+      <c r="B83" s="83" t="s">
         <v>176</v>
       </c>
-      <c r="C83" s="85" t="s">
+      <c r="C83" s="84" t="s">
         <v>214</v>
       </c>
-      <c r="D83" s="86">
+      <c r="D83" s="85">
         <f>VLOOKUP($A83,import!$A:$G,MATCH(lookup_helper!D$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>1.3624389724527719</v>
       </c>
-      <c r="E83" s="86">
+      <c r="E83" s="85">
         <f>VLOOKUP($A83,import!$A:$G,MATCH(lookup_helper!E$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
-      <c r="F83" s="86">
+      <c r="F83" s="85">
         <f>VLOOKUP($A83,import!$A:$G,MATCH(lookup_helper!F$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="G83" s="86">
+      <c r="G83" s="85">
         <f>VLOOKUP($A83,import!$A:$G,MATCH(lookup_helper!G$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0.19527333899999999</v>
       </c>
-      <c r="H83" s="86">
+      <c r="H83" s="85">
         <f>VLOOKUP($A83,import!$A:$G,MATCH(lookup_helper!H$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I83" s="86">
+      <c r="I83" s="85">
         <f>VLOOKUP($A83,import!$A:$G,MATCH(lookup_helper!I$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:16" s="85" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="83" t="s">
+    <row r="84" spans="1:16" s="84" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="82" t="s">
         <v>66</v>
       </c>
-      <c r="B84" s="84" t="s">
+      <c r="B84" s="83" t="s">
         <v>177</v>
       </c>
-      <c r="C84" s="85" t="s">
+      <c r="C84" s="84" t="s">
         <v>214</v>
       </c>
-      <c r="D84" s="86">
+      <c r="D84" s="85">
         <f>VLOOKUP($A84,import!$A:$G,MATCH(lookup_helper!D$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>1.475654647382425</v>
       </c>
-      <c r="E84" s="86">
+      <c r="E84" s="85">
         <f>VLOOKUP($A84,import!$A:$G,MATCH(lookup_helper!E$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
-      <c r="F84" s="86">
+      <c r="F84" s="85">
         <f>VLOOKUP($A84,import!$A:$G,MATCH(lookup_helper!F$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>2.6</v>
       </c>
-      <c r="G84" s="86">
+      <c r="G84" s="85">
         <f>VLOOKUP($A84,import!$A:$G,MATCH(lookup_helper!G$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0.18979411900000001</v>
       </c>
-      <c r="H84" s="86">
+      <c r="H84" s="85">
         <f>VLOOKUP($A84,import!$A:$G,MATCH(lookup_helper!H$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
-      <c r="I84" s="86">
+      <c r="I84" s="85">
         <f>VLOOKUP($A84,import!$A:$G,MATCH(lookup_helper!I$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
@@ -22436,19 +22436,19 @@
       <c r="C87" t="s">
         <v>205</v>
       </c>
-      <c r="D87" s="92">
+      <c r="D87" s="91">
         <f>VLOOKUP($A87,import!$A:$G,MATCH(lookup_helper!D$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>41.285465803940781</v>
       </c>
-      <c r="E87" s="92">
+      <c r="E87" s="91">
         <f>VLOOKUP($A87,import!$A:$G,MATCH(lookup_helper!E$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
-      <c r="F87" s="92">
+      <c r="F87" s="91">
         <f>VLOOKUP($A87,import!$A:$G,MATCH(lookup_helper!F$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>61.135362311155802</v>
       </c>
-      <c r="G87" s="92">
+      <c r="G87" s="91">
         <f>VLOOKUP($A87,import!$A:$G,MATCH(lookup_helper!G$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>63.369834818958772</v>
       </c>
@@ -22506,19 +22506,19 @@
       <c r="C89" t="s">
         <v>205</v>
       </c>
-      <c r="D89" s="92">
+      <c r="D89" s="91">
         <f>VLOOKUP($A89,import!$A:$G,MATCH(lookup_helper!D$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>1.474480921569314</v>
       </c>
-      <c r="E89" s="92">
+      <c r="E89" s="91">
         <f>VLOOKUP($A89,import!$A:$G,MATCH(lookup_helper!E$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>0</v>
       </c>
-      <c r="F89" s="92">
+      <c r="F89" s="91">
         <f>VLOOKUP($A89,import!$A:$G,MATCH(lookup_helper!F$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>1.6732642555122741</v>
       </c>
-      <c r="G89" s="92">
+      <c r="G89" s="91">
         <f>VLOOKUP($A89,import!$A:$G,MATCH(lookup_helper!G$1,import!$A$1:$G$1,0),FALSE)</f>
         <v>1.2819088722919141</v>
       </c>
@@ -23676,88 +23676,88 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="81" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="159" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="97" t="s">
+      <c r="A6" s="96" t="s">
         <v>307</v>
       </c>
-      <c r="B6" s="97"/>
-      <c r="C6" s="97"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="97"/>
-      <c r="H6" s="97"/>
-      <c r="I6" s="97"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="96"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="82" t="s">
+      <c r="A9" s="81" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="97" t="s">
+      <c r="A10" s="96" t="s">
         <v>308</v>
       </c>
-      <c r="B10" s="97"/>
-      <c r="C10" s="97"/>
-      <c r="D10" s="97"/>
-      <c r="E10" s="97"/>
-      <c r="F10" s="97"/>
-      <c r="G10" s="97"/>
-      <c r="H10" s="97"/>
-      <c r="I10" s="97"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="96"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="96"/>
+      <c r="I10" s="96"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="69"/>
-      <c r="B28" s="69"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
+      <c r="A28" s="68"/>
+      <c r="B28" s="68"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
       <c r="E28" s="31"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="79"/>
+      <c r="A29" s="78"/>
       <c r="E29" s="31"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="69"/>
-      <c r="B30" s="69"/>
-      <c r="C30" s="69"/>
-      <c r="D30" s="69"/>
+      <c r="A30" s="68"/>
+      <c r="B30" s="68"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="68"/>
       <c r="E30" s="31"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="69"/>
-      <c r="B31" s="69"/>
-      <c r="C31" s="69"/>
-      <c r="D31" s="69"/>
+      <c r="A31" s="68"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="68"/>
       <c r="E31" s="31"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="69"/>
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69"/>
+      <c r="A32" s="68"/>
+      <c r="B32" s="68"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="68"/>
       <c r="E32" s="32"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="69"/>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
+      <c r="A33" s="68"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="68"/>
       <c r="E33" s="48"/>
       <c r="F33" s="30"/>
       <c r="G33" s="30"/>
@@ -23815,7 +23815,7 @@
       <c r="I38" s="11"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="56"/>
+      <c r="A39" s="55"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
@@ -23826,7 +23826,7 @@
       <c r="I39" s="11"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="57"/>
+      <c r="A40" s="56"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
@@ -23874,13 +23874,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H1" s="68" t="str">
+      <c r="H1" s="67" t="str">
         <f>"Project name: "&amp;VLOOKUP("Project name",lookup_helper!$B:$D,3,FALSE)</f>
         <v>Project name: test_project_YubaCity</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H2" s="68" t="str">
+      <c r="H2" s="67" t="str">
         <f>"Project community type: "&amp;VLOOKUP("Project Community Type",lookup_helper!$B:$D,3,FALSE)</f>
         <v>Project community type: Small-Town Established Communities</v>
       </c>
@@ -23904,45 +23904,45 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="88"/>
-      <c r="C42" s="88"/>
-      <c r="D42" s="88"/>
-      <c r="E42" s="88"/>
-      <c r="F42" s="88"/>
-      <c r="G42" s="88"/>
-      <c r="H42" s="88"/>
+      <c r="B42" s="87"/>
+      <c r="C42" s="87"/>
+      <c r="D42" s="87"/>
+      <c r="E42" s="87"/>
+      <c r="F42" s="87"/>
+      <c r="G42" s="87"/>
+      <c r="H42" s="87"/>
     </row>
     <row r="43" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="98" t="s">
+      <c r="A43" s="97" t="s">
         <v>268</v>
       </c>
-      <c r="B43" s="98"/>
-      <c r="C43" s="98"/>
-      <c r="D43" s="98"/>
-      <c r="E43" s="98"/>
-      <c r="F43" s="98"/>
-      <c r="G43" s="98"/>
-      <c r="H43" s="98"/>
+      <c r="B43" s="97"/>
+      <c r="C43" s="97"/>
+      <c r="D43" s="97"/>
+      <c r="E43" s="97"/>
+      <c r="F43" s="97"/>
+      <c r="G43" s="97"/>
+      <c r="H43" s="97"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="88"/>
-      <c r="B44" s="88"/>
-      <c r="C44" s="88"/>
-      <c r="D44" s="88"/>
-      <c r="E44" s="88"/>
-      <c r="F44" s="88"/>
-      <c r="G44" s="88"/>
-      <c r="H44" s="88"/>
+      <c r="A44" s="87"/>
+      <c r="B44" s="87"/>
+      <c r="C44" s="87"/>
+      <c r="D44" s="87"/>
+      <c r="E44" s="87"/>
+      <c r="F44" s="87"/>
+      <c r="G44" s="87"/>
+      <c r="H44" s="87"/>
     </row>
     <row r="45" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="88"/>
-      <c r="B45" s="88"/>
-      <c r="C45" s="88"/>
-      <c r="D45" s="88"/>
-      <c r="E45" s="88"/>
-      <c r="F45" s="88"/>
-      <c r="G45" s="88"/>
-      <c r="H45" s="88"/>
+      <c r="A45" s="87"/>
+      <c r="B45" s="87"/>
+      <c r="C45" s="87"/>
+      <c r="D45" s="87"/>
+      <c r="E45" s="87"/>
+      <c r="F45" s="87"/>
+      <c r="G45" s="87"/>
+      <c r="H45" s="87"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="29" t="s">
@@ -23950,16 +23950,16 @@
       </c>
     </row>
     <row r="67" spans="1:8" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="99" t="s">
+      <c r="A67" s="98" t="s">
         <v>296</v>
       </c>
-      <c r="B67" s="99"/>
-      <c r="C67" s="99"/>
-      <c r="D67" s="99"/>
-      <c r="E67" s="99"/>
-      <c r="F67" s="99"/>
-      <c r="G67" s="99"/>
-      <c r="H67" s="99"/>
+      <c r="B67" s="98"/>
+      <c r="C67" s="98"/>
+      <c r="D67" s="98"/>
+      <c r="E67" s="98"/>
+      <c r="F67" s="98"/>
+      <c r="G67" s="98"/>
+      <c r="H67" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -23987,20 +23987,20 @@
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H1" s="68" t="str">
+    <row r="1" spans="1:8" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="67" t="str">
         <f>"Project name: "&amp;VLOOKUP("Project name",lookup_helper!$B:$D,3,FALSE)</f>
         <v>Project name: test_project_YubaCity</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H2" s="68" t="str">
+    <row r="2" spans="1:8" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="67" t="str">
         <f>"Project community type: "&amp;VLOOKUP("Project Community Type",lookup_helper!$B:$D,3,FALSE)</f>
         <v>Project community type: Small-Town Established Communities</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="58"/>
+      <c r="A3" s="57"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -24037,131 +24037,131 @@
       <c r="A13" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="76" t="s">
+      <c r="A22" s="75" t="s">
         <v>284</v>
       </c>
-      <c r="B22" s="74" t="str">
+      <c r="B22" s="73" t="str">
         <f>lookup_helper!Q7</f>
         <v>EB</v>
       </c>
-      <c r="C22" s="74" t="str">
+      <c r="C22" s="73" t="str">
         <f>lookup_helper!R7</f>
         <v>WB</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="75" t="s">
+      <c r="A23" s="74" t="s">
         <v>286</v>
       </c>
-      <c r="B23" s="78">
+      <c r="B23" s="77">
         <f>IFERROR(lookup_helper!Q9/lookup_helper!Q8,0)</f>
         <v>0.62906584321456371</v>
       </c>
-      <c r="C23" s="78">
+      <c r="C23" s="77">
         <f>IFERROR(lookup_helper!R9/lookup_helper!R8,0)</f>
         <v>0.81902208942477273</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="79" t="s">
+      <c r="A25" s="78" t="s">
         <v>131</v>
       </c>
-      <c r="C25" s="71"/>
+      <c r="C25" s="70"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="80">
+      <c r="A26" s="79">
         <f>VLOOKUP(A25,lookup_helper!$B:$D,3,FALSE)</f>
         <v>60000</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D27" s="72"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
-      <c r="G27" s="72"/>
-      <c r="H27" s="72"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="71"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="70"/>
-      <c r="B28" s="73"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="72"/>
-      <c r="G28" s="72"/>
-      <c r="H28" s="72"/>
+      <c r="A28" s="69"/>
+      <c r="B28" s="72"/>
+      <c r="C28" s="72"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
     </row>
     <row r="29" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="99" t="s">
+      <c r="A29" s="98" t="s">
         <v>293</v>
       </c>
-      <c r="B29" s="99"/>
-      <c r="C29" s="99"/>
-      <c r="D29" s="99"/>
-      <c r="E29" s="99"/>
-      <c r="F29" s="99"/>
-      <c r="G29" s="99"/>
-      <c r="H29" s="99"/>
+      <c r="B29" s="98"/>
+      <c r="C29" s="98"/>
+      <c r="D29" s="98"/>
+      <c r="E29" s="98"/>
+      <c r="F29" s="98"/>
+      <c r="G29" s="98"/>
+      <c r="H29" s="98"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="72"/>
-      <c r="B31" s="72"/>
-      <c r="C31" s="72"/>
-      <c r="D31" s="72"/>
-      <c r="E31" s="72"/>
-      <c r="F31" s="72"/>
-      <c r="G31" s="72"/>
-      <c r="H31" s="72"/>
+      <c r="A31" s="71"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="71"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="71"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="72"/>
-      <c r="B32" s="72"/>
-      <c r="C32" s="72"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="72"/>
-      <c r="F32" s="72"/>
-      <c r="G32" s="72"/>
-      <c r="H32" s="72"/>
+      <c r="A32" s="71"/>
+      <c r="B32" s="71"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="71"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="71"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="72"/>
-      <c r="B33" s="72"/>
-      <c r="C33" s="72"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="72"/>
-      <c r="G33" s="72"/>
-      <c r="H33" s="72"/>
+      <c r="A33" s="71"/>
+      <c r="B33" s="71"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="72"/>
-      <c r="B34" s="72"/>
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="72"/>
-      <c r="F34" s="72"/>
-      <c r="G34" s="72"/>
-      <c r="H34" s="72"/>
+      <c r="A34" s="71"/>
+      <c r="B34" s="71"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="71"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="72"/>
-      <c r="B35" s="72"/>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
-      <c r="F35" s="72"/>
-      <c r="G35" s="72"/>
-      <c r="H35" s="72"/>
+      <c r="A35" s="71"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="71"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="72"/>
-      <c r="B36" s="72"/>
-      <c r="C36" s="72"/>
-      <c r="D36" s="72"/>
-      <c r="E36" s="72"/>
-      <c r="F36" s="72"/>
-      <c r="G36" s="72"/>
-      <c r="H36" s="72"/>
+      <c r="A36" s="71"/>
+      <c r="B36" s="71"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="71"/>
+      <c r="E36" s="71"/>
+      <c r="F36" s="71"/>
+      <c r="G36" s="71"/>
+      <c r="H36" s="71"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
@@ -24169,16 +24169,16 @@
       </c>
     </row>
     <row r="62" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="99" t="s">
+      <c r="A62" s="98" t="s">
         <v>275</v>
       </c>
-      <c r="B62" s="99"/>
-      <c r="C62" s="99"/>
-      <c r="D62" s="99"/>
-      <c r="E62" s="99"/>
-      <c r="F62" s="99"/>
-      <c r="G62" s="99"/>
-      <c r="H62" s="99"/>
+      <c r="B62" s="98"/>
+      <c r="C62" s="98"/>
+      <c r="D62" s="98"/>
+      <c r="E62" s="98"/>
+      <c r="F62" s="98"/>
+      <c r="G62" s="98"/>
+      <c r="H62" s="98"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="29"/>
@@ -24202,7 +24202,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView view="pageLayout" topLeftCell="A31" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -24215,20 +24215,20 @@
     <col min="8" max="8" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H1" s="68" t="str">
+    <row r="1" spans="1:9" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="67" t="str">
         <f>"Project name: "&amp;VLOOKUP("Project name",lookup_helper!$B:$D,3,FALSE)</f>
         <v>Project name: test_project_YubaCity</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H2" s="68" t="str">
+    <row r="2" spans="1:9" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="67" t="str">
         <f>"Project community type: "&amp;VLOOKUP("Project Community Type",lookup_helper!$B:$D,3,FALSE)</f>
         <v>Project community type: Small-Town Established Communities</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
+      <c r="A3" s="58"/>
     </row>
     <row r="4" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -24236,13 +24236,13 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="99" t="s">
         <v>224</v>
       </c>
-      <c r="B5" s="100"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="99"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="41" t="s">
@@ -24280,24 +24280,24 @@
       <c r="C10" s="39"/>
     </row>
     <row r="12" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="100" t="s">
+      <c r="A12" s="99" t="s">
         <v>225</v>
       </c>
-      <c r="B12" s="100"/>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="100"/>
+      <c r="B12" s="99"/>
+      <c r="C12" s="99"/>
+      <c r="D12" s="99"/>
+      <c r="E12" s="99"/>
       <c r="F12" s="36"/>
       <c r="G12" s="36"/>
       <c r="H12" s="36"/>
       <c r="I12" s="36"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="101" t="s">
+      <c r="A14" s="100" t="s">
         <v>235</v>
       </c>
-      <c r="B14" s="101"/>
-      <c r="C14" s="101"/>
+      <c r="B14" s="100"/>
+      <c r="C14" s="100"/>
     </row>
     <row r="15" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="34" t="s">
@@ -24427,7 +24427,7 @@
   <dimension ref="A1:H69"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H2"/>
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24435,20 +24435,20 @@
     <col min="8" max="8" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H1" s="68" t="str">
+    <row r="1" spans="1:8" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="67" t="str">
         <f>"Project name: "&amp;VLOOKUP("Project name",lookup_helper!$B:$D,3,FALSE)</f>
         <v>Project name: test_project_YubaCity</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H2" s="68" t="str">
+    <row r="2" spans="1:8" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="67" t="str">
         <f>"Project community type: "&amp;VLOOKUP("Project Community Type",lookup_helper!$B:$D,3,FALSE)</f>
         <v>Project community type: Small-Town Established Communities</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
+      <c r="A3" s="58"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -24456,26 +24456,26 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="102" t="s">
+      <c r="A5" s="101" t="s">
         <v>285</v>
       </c>
-      <c r="B5" s="102"/>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="102"/>
-      <c r="H5" s="102"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="87"/>
-      <c r="B6" s="87"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
+      <c r="A6" s="86"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="29"/>
@@ -24528,7 +24528,8 @@
       </c>
     </row>
     <row r="46" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="54">
+      <c r="A46" s="103">
+        <f>VLOOKUP("K-12 school enrollment",lookup_helper!$B:$D,3,FALSE)</f>
         <v>657</v>
       </c>
     </row>
@@ -24538,10 +24539,10 @@
       </c>
     </row>
     <row r="64" spans="1:1" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="89"/>
+      <c r="A64" s="88"/>
     </row>
     <row r="65" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="90"/>
+      <c r="A65" s="89"/>
     </row>
     <row r="66" spans="1:1" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="67" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
@@ -24587,20 +24588,20 @@
     <col min="9" max="9" width="5.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H1" s="68" t="str">
+    <row r="1" spans="1:9" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="67" t="str">
         <f>"Project name: "&amp;VLOOKUP("Project name",lookup_helper!$B:$D,3,FALSE)</f>
         <v>Project name: test_project_YubaCity</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H2" s="68" t="str">
+    <row r="2" spans="1:9" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="67" t="str">
         <f>"Project community type: "&amp;VLOOKUP("Project Community Type",lookup_helper!$B:$D,3,FALSE)</f>
         <v>Project community type: Small-Town Established Communities</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
+      <c r="A3" s="58"/>
     </row>
     <row r="4" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -24608,17 +24609,17 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="102" t="s">
         <v>269</v>
       </c>
-      <c r="B5" s="103"/>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
-      <c r="E5" s="103"/>
-      <c r="F5" s="103"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="55"/>
+      <c r="B5" s="102"/>
+      <c r="C5" s="102"/>
+      <c r="D5" s="102"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="102"/>
+      <c r="I5" s="54"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="45">
@@ -24646,17 +24647,17 @@
       <c r="I7" s="31"/>
     </row>
     <row r="8" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="98" t="s">
+      <c r="A8" s="97" t="s">
         <v>240</v>
       </c>
-      <c r="B8" s="98"/>
-      <c r="C8" s="98"/>
-      <c r="D8" s="98"/>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="98"/>
-      <c r="H8" s="98"/>
-      <c r="I8" s="55"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="97"/>
+      <c r="G8" s="97"/>
+      <c r="H8" s="97"/>
+      <c r="I8" s="54"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
@@ -24731,20 +24732,20 @@
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H1" s="68" t="str">
+    <row r="1" spans="1:8" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="67" t="str">
         <f>"Project name: "&amp;VLOOKUP("Project name",lookup_helper!$B:$D,3,FALSE)</f>
         <v>Project name: test_project_YubaCity</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H2" s="68" t="str">
+    <row r="2" spans="1:8" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="67" t="str">
         <f>"Project community type: "&amp;VLOOKUP("Project Community Type",lookup_helper!$B:$D,3,FALSE)</f>
         <v>Project community type: Small-Town Established Communities</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
+      <c r="A3" s="58"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -24752,16 +24753,16 @@
       </c>
     </row>
     <row r="5" spans="1:8" s="28" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="98" t="s">
+      <c r="A5" s="97" t="s">
         <v>245</v>
       </c>
-      <c r="B5" s="98"/>
-      <c r="C5" s="98"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="98"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="97"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
@@ -24838,7 +24839,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="79" t="s">
+      <c r="A70" s="78" t="s">
         <v>302</v>
       </c>
     </row>
@@ -24892,20 +24893,20 @@
     <col min="8" max="8" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H1" s="68" t="str">
+    <row r="1" spans="1:8" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="67" t="str">
         <f>"Project name: "&amp;VLOOKUP("Project name",lookup_helper!$B:$D,3,FALSE)</f>
         <v>Project name: test_project_YubaCity</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="66" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H2" s="68" t="str">
+    <row r="2" spans="1:8" s="65" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="67" t="str">
         <f>"Project community type: "&amp;VLOOKUP("Project Community Type",lookup_helper!$B:$D,3,FALSE)</f>
         <v>Project community type: Small-Town Established Communities</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
+      <c r="A3" s="58"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -24940,22 +24941,22 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="93">
+      <c r="A14" s="92">
         <f>VLOOKUP("Complete street score",lookup_helper!$B:$D,3,FALSE)</f>
         <v>-1</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="163.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="103" t="s">
+      <c r="A16" s="102" t="s">
         <v>300</v>
       </c>
-      <c r="B16" s="103"/>
-      <c r="C16" s="103"/>
-      <c r="D16" s="103"/>
-      <c r="E16" s="103"/>
-      <c r="F16" s="103"/>
-      <c r="G16" s="103"/>
-      <c r="H16" s="103"/>
+      <c r="B16" s="102"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="102"/>
+      <c r="H16" s="102"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>